<commit_message>
Milestone 1, 30 oktober 2016
</commit_message>
<xml_diff>
--- a/Milestone 1/Milestone 1 - Timesheet.xlsx
+++ b/Milestone 1/Milestone 1 - Timesheet.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\adriglib.github.io\Milestone 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\GDM\NWDAD II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19188" windowHeight="6708"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet Adriaan Glibert" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="37">
   <si>
     <t>Datum</t>
   </si>
@@ -129,12 +129,18 @@
   </si>
   <si>
     <t>Taak</t>
+  </si>
+  <si>
+    <t>29.10.2016</t>
+  </si>
+  <si>
+    <t>Aanpassen aan feedback</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General\ &quot;uur&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;Som:&quot;\ General\ &quot;uur&quot;"/>
@@ -180,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -210,7 +216,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -304,6 +309,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -339,6 +361,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -493,18 +532,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="40.625" customWidth="1"/>
-    <col min="4" max="4" width="48.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.625" customWidth="1"/>
+    <col min="1" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -522,7 +561,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -530,7 +569,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -548,7 +587,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -566,7 +605,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -584,7 +623,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -602,7 +641,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -620,7 +659,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
@@ -638,7 +677,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -656,7 +695,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -674,7 +713,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -692,7 +731,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -710,7 +749,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -728,7 +767,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -746,7 +785,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -764,7 +803,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
@@ -782,7 +821,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -800,7 +839,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -818,21 +857,25 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.45">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="11">
-        <f ca="1">TODAY()</f>
-        <v>42665</v>
-      </c>
-      <c r="E19" s="7">
-        <f>SUM(E3:E18)</f>
-        <v>23.25</v>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="9">
+        <v>2</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -840,7 +883,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -848,7 +891,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -856,15 +899,18 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="23.4" x14ac:dyDescent="0.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="7">
+        <f>SUM(E3:E19)</f>
+        <v>25.25</v>
+      </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -872,7 +918,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>

</xml_diff>